<commit_message>
regular commit, end of the day
</commit_message>
<xml_diff>
--- a/media/excel_template/fp_temp.xlsx
+++ b/media/excel_template/fp_temp.xlsx
@@ -3229,31 +3229,6 @@
     </pic>
     <clientData/>
   </twoCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>7</col>
-      <colOff>304919</colOff>
-      <row>22</row>
-      <rowOff>90490</rowOff>
-    </from>
-    <ext cx="2514600" cy="2333625"/>
-    <pic>
-      <nvPicPr>
-        <cNvPr id="2" name="Image 2" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:fillRect/>
-        </a:stretch>
-      </blipFill>
-      <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
-      </spPr>
-    </pic>
-    <clientData/>
-  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -3716,11 +3691,7 @@
       </c>
       <c r="E2" s="174" t="n"/>
       <c r="F2" s="196" t="n"/>
-      <c r="G2" s="197" t="inlineStr">
-        <is>
-          <t>MACHINE D'EXERCICE POUR L'ENTRAINEMENT DES MUSCLES DU MOLLET</t>
-        </is>
-      </c>
+      <c r="G2" s="197" t="inlineStr"/>
       <c r="H2" s="179" t="n"/>
       <c r="I2" s="179" t="n"/>
       <c r="J2" s="179" t="n"/>
@@ -3757,11 +3728,7 @@
       </c>
       <c r="E3" s="183" t="n"/>
       <c r="F3" s="199" t="n"/>
-      <c r="G3" s="200" t="inlineStr">
-        <is>
-          <t>ТРЕНАЖЕР ДЛЯ ТРЕНИРОВКИ ИКРОНОЖНЫХ МЫШЦ</t>
-        </is>
-      </c>
+      <c r="G3" s="200" t="inlineStr"/>
       <c r="H3" s="201" t="n"/>
       <c r="I3" s="201" t="n"/>
       <c r="J3" s="201" t="n"/>
@@ -3805,18 +3772,14 @@
       </c>
       <c r="B4" s="174" t="n"/>
       <c r="C4" s="174" t="n"/>
-      <c r="D4" s="175" t="n">
-        <v>15</v>
-      </c>
+      <c r="D4" s="175" t="n"/>
       <c r="E4" s="177" t="inlineStr">
         <is>
           <t xml:space="preserve">Chantier:  </t>
         </is>
       </c>
       <c r="F4" s="174" t="n"/>
-      <c r="G4" s="178" t="n">
-        <v>2</v>
-      </c>
+      <c r="G4" s="178" t="n"/>
       <c r="H4" s="179" t="n"/>
       <c r="I4" s="179" t="n"/>
       <c r="J4" s="179" t="n"/>
@@ -3881,9 +3844,7 @@
       </c>
       <c r="B6" s="160" t="n"/>
       <c r="C6" s="160" t="n"/>
-      <c r="D6" s="226" t="n">
-        <v>1</v>
-      </c>
+      <c r="D6" s="226" t="n"/>
       <c r="E6" s="219" t="n"/>
       <c r="F6" s="223" t="n"/>
       <c r="G6" s="227" t="inlineStr">
@@ -3894,9 +3855,7 @@
       <c r="H6" s="219" t="n"/>
       <c r="I6" s="219" t="n"/>
       <c r="J6" s="223" t="n"/>
-      <c r="K6" s="222" t="n">
-        <v>2</v>
-      </c>
+      <c r="K6" s="222" t="n"/>
       <c r="L6" s="219" t="n"/>
       <c r="M6" s="219" t="n"/>
       <c r="N6" s="219" t="n"/>
@@ -3909,9 +3868,7 @@
       </c>
       <c r="R6" s="160" t="n"/>
       <c r="S6" s="161" t="n"/>
-      <c r="T6" s="222" t="n">
-        <v>1</v>
-      </c>
+      <c r="T6" s="222" t="n"/>
       <c r="U6" s="219" t="n"/>
       <c r="V6" s="219" t="n"/>
       <c r="W6" s="219" t="n"/>
@@ -3982,9 +3939,7 @@
       </c>
       <c r="B8" s="160" t="n"/>
       <c r="C8" s="161" t="n"/>
-      <c r="D8" s="209" t="n">
-        <v>1</v>
-      </c>
+      <c r="D8" s="209" t="n"/>
       <c r="E8" s="210" t="n"/>
       <c r="F8" s="210" t="n"/>
       <c r="G8" s="210" t="n"/>
@@ -4115,12 +4070,7 @@
       <c r="AJ10" s="220" t="n"/>
     </row>
     <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="255" t="inlineStr">
-        <is>
-          <t>"MACHINE D'EXERCICE POUR L'ENTRAINEMENT DES MUSCLES DU MOLLET                                                                                                Entraîne efficacement et en toute sécurité les muscles du mollet. À cet égard, le coussin de siège de forme anatomique ainsi que le siège en luge réglable pour une adaptation de la longueur des jambes garantissent toujours une biomécanique optimale. Grâce à la position du siège, la colonne vertébrale est déchargée. Tout cela garantit un entraînement confortable et sûr. Ceci est confirmé et documenté par l'homologation de la machine en tant que ""produit médical"" conformément à MPG.                             
-Qté:1"</t>
-        </is>
-      </c>
+      <c r="A11" s="255" t="inlineStr"/>
       <c r="B11" s="256" t="n"/>
       <c r="C11" s="256" t="n"/>
       <c r="D11" s="256" t="n"/>
@@ -4132,14 +4082,7 @@
       <c r="J11" s="256" t="n"/>
       <c r="K11" s="257" t="n"/>
       <c r="L11" s="98" t="n"/>
-      <c r="M11" s="260" t="inlineStr">
-        <is>
-          <t>"ТРЕНАЖЕР ДЛЯ ТРЕНИРОВКИ ИКРОНОЖНЫХ МЫШЦ
-Эффективно и безопасно тренирует икроножные мышцы. В этом отношении подушка сиденья анатомической формы и регулируемое сиденье салазок для адаптации длины ноги всегда гарантируют оптимальную биомеханику. Из-за положения сиденья позвоночник разгружен. Все это гарантирует комфортную и безопасную тренировку. Это подтверждается и документируется утверждением машины как «медицинского продукта» согласно MPG.
-Кол-во: 1 шт             
-"</t>
-        </is>
-      </c>
+      <c r="M11" s="260" t="inlineStr"/>
       <c r="N11" s="256" t="n"/>
       <c r="O11" s="256" t="n"/>
       <c r="P11" s="256" t="n"/>
@@ -4735,7 +4678,7 @@
       <c r="B29" s="160" t="n"/>
       <c r="C29" s="160" t="n"/>
       <c r="D29" s="217" t="n"/>
-      <c r="E29" s="242" t="n"/>
+      <c r="E29" s="242" t="inlineStr"/>
       <c r="F29" s="219" t="n"/>
       <c r="G29" s="219" t="n"/>
       <c r="H29" s="219" t="n"/>
@@ -4814,7 +4757,7 @@
       <c r="B31" s="160" t="n"/>
       <c r="C31" s="160" t="n"/>
       <c r="D31" s="160" t="n"/>
-      <c r="E31" s="242" t="n"/>
+      <c r="E31" s="242" t="inlineStr"/>
       <c r="F31" s="219" t="n"/>
       <c r="G31" s="219" t="n"/>
       <c r="H31" s="219" t="n"/>
@@ -5392,14 +5335,10 @@
       <c r="B45" s="297" t="n"/>
       <c r="C45" s="297" t="n"/>
       <c r="D45" s="298" t="n"/>
-      <c r="E45" s="163" t="n">
-        <v>1</v>
-      </c>
+      <c r="E45" s="163" t="n"/>
       <c r="F45" s="164" t="n"/>
       <c r="G45" s="165" t="n"/>
-      <c r="H45" s="299" t="n">
-        <v>15</v>
-      </c>
+      <c r="H45" s="299" t="n"/>
       <c r="I45" s="298" t="n"/>
       <c r="J45" s="166" t="n"/>
       <c r="K45" s="164" t="n"/>
@@ -5409,20 +5348,12 @@
       <c r="O45" s="168" t="n"/>
       <c r="P45" s="169" t="n"/>
       <c r="Q45" s="168" t="n"/>
-      <c r="R45" s="167" t="inlineStr">
-        <is>
-          <t>FPCRI0001</t>
-        </is>
-      </c>
+      <c r="R45" s="167" t="inlineStr"/>
       <c r="S45" s="301" t="n"/>
       <c r="T45" s="301" t="n"/>
       <c r="U45" s="301" t="n"/>
       <c r="V45" s="168" t="n"/>
-      <c r="W45" s="300" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
+      <c r="W45" s="300" t="inlineStr"/>
       <c r="X45" s="301" t="n"/>
       <c r="Y45" s="302" t="n"/>
       <c r="Z45" s="283" t="n"/>

</xml_diff>

<commit_message>
now annexe5 and room can be added to fiche produits
</commit_message>
<xml_diff>
--- a/media/excel_template/fp_temp.xlsx
+++ b/media/excel_template/fp_temp.xlsx
@@ -3718,7 +3718,7 @@
       <c r="F2" s="196" t="n"/>
       <c r="G2" s="197" t="inlineStr">
         <is>
-          <t>Simulateur à câble</t>
+          <t>SIMULATEUR DE LEVAGE DE LA PAZ</t>
         </is>
       </c>
       <c r="H2" s="179" t="n"/>
@@ -3759,7 +3759,7 @@
       <c r="F3" s="199" t="n"/>
       <c r="G3" s="200" t="inlineStr">
         <is>
-          <t>Тросовый тренажер</t>
+          <t>ТРЕНАЖЕР ДЛЯ ПОДЪЕМА ТАЗА</t>
         </is>
       </c>
       <c r="H3" s="201" t="n"/>
@@ -3806,7 +3806,7 @@
       <c r="B4" s="174" t="n"/>
       <c r="C4" s="174" t="n"/>
       <c r="D4" s="175" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E4" s="177" t="inlineStr">
         <is>
@@ -3882,7 +3882,7 @@
       <c r="B6" s="160" t="n"/>
       <c r="C6" s="160" t="n"/>
       <c r="D6" s="226" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E6" s="219" t="n"/>
       <c r="F6" s="223" t="n"/>
@@ -3982,8 +3982,10 @@
       </c>
       <c r="B8" s="160" t="n"/>
       <c r="C8" s="161" t="n"/>
-      <c r="D8" s="209" t="n">
-        <v>4</v>
+      <c r="D8" s="209" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
       </c>
       <c r="E8" s="210" t="n"/>
       <c r="F8" s="210" t="n"/>
@@ -4117,15 +4119,13 @@
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="255" t="inlineStr">
         <is>
-          <t>"Simulateur à câble
-Dimensions 96 x 105 x 201 cm
-Poids 200 kg
-Poids standard: 55 kg (disponible en 70 et 105 kg) - intervalle d'ajustement de la résistance de 5 kg
-Libre sur le sol, peut être utilisé sans banc fixe
-La taille est ajustable à la taille de la poutre
-Peut être utilisé seul ou à deux mains
-Egalement disponible avec 1 kg de poids supplémentaire par incréments de 1 kg (2-7pcs / pc / accessoire)
-La hauteur des appareils est personnalisable
+          <t>"SIMULATEUR DE LEVAGE DE LA PAZ
+Entraîne les muscles extenseurs de manière sûre et efficace en position horizontale. Le coussin rond parfaitement formé et ajustable ainsi que le réglage individuel de la longueur des jambes créent une situation optimale pour l’entraînement.
+Hauteur: 1570 mm
+Largeur: 1200 mm
+Longueur: 1800 mm
+Poids total 290.00 kg
+Bloc de poids standard 60 kg
 Qty: 1 U"</t>
         </is>
       </c>
@@ -4142,15 +4142,13 @@
       <c r="L11" s="98" t="n"/>
       <c r="M11" s="260" t="inlineStr">
         <is>
-          <t>"Тросовый тренажер
-Размеры 96 х 105 х 201 см
-Вес 200 кг
-Стандартный весовой пакет: 55 кг (в наличии 70 и 105 кг) - интервал регулировки сопротивления 5 кг
-Свободно на полу, можно использовать без неподвижной скамьи
-Талия регулируется по размеру всего луча
-Может использоваться как одноручный или двуручный
-Также доступны с дополнительным весом 1 кг с шагом 1 кг (2-7 шт. / Шт. / Аксессуар)
-Высота устройств настраивается
+          <t>"ТРЕНАЖЕР ДЛЯ ПОДЪЕМА ТАЗА
+Тренирует мышцы-разгибатели безопасно и эффективно в горизонтальном положении. Идеальная форма и регулируемая круглая подушка, а также индивидуальная регулировка длины ног создают оптимальную тренировочную ситуацию.
+Высота: 1570 мм
+Ширина: 1200 мм
+Длина: 1800 мм
+Общий вес 290,00 кг
+Стандартный вес блока 60 кг
 Кол-во: 1 шт"</t>
         </is>
       </c>
@@ -5420,7 +5418,7 @@
       <c r="F45" s="164" t="n"/>
       <c r="G45" s="165" t="n"/>
       <c r="H45" s="299" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="I45" s="298" t="n"/>
       <c r="J45" s="166" t="n"/>
@@ -5433,7 +5431,7 @@
       <c r="Q45" s="168" t="n"/>
       <c r="R45" s="167" t="inlineStr">
         <is>
-          <t>FP00001</t>
+          <t>04003</t>
         </is>
       </c>
       <c r="S45" s="301" t="n"/>

</xml_diff>

<commit_message>
fiche produit print page is ongoing
</commit_message>
<xml_diff>
--- a/media/excel_template/fp_temp.xlsx
+++ b/media/excel_template/fp_temp.xlsx
@@ -3236,7 +3236,7 @@
       <row>22</row>
       <rowOff>90490</rowOff>
     </from>
-    <ext cx="2762250" cy="2333625"/>
+    <ext cx="2895600" cy="2333625"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -3718,7 +3718,7 @@
       <c r="F2" s="196" t="n"/>
       <c r="G2" s="197" t="inlineStr">
         <is>
-          <t>SIMULATEUR DE LEVAGE DE LA PAZ</t>
+          <t>RACK POUR LES GRIFFE EXCLUSIVES RAUSCHENBACH</t>
         </is>
       </c>
       <c r="H2" s="179" t="n"/>
@@ -3759,7 +3759,7 @@
       <c r="F3" s="199" t="n"/>
       <c r="G3" s="200" t="inlineStr">
         <is>
-          <t>ТРЕНАЖЕР ДЛЯ ПОДЪЕМА ТАЗА</t>
+          <t>СТОЙКА ДЛЯ ГРИФОВ ЭКСКЛЮЗИВНОЙ КОНСТРУКЦИИ RAUSCHENBACH</t>
         </is>
       </c>
       <c r="H3" s="201" t="n"/>
@@ -3806,7 +3806,7 @@
       <c r="B4" s="174" t="n"/>
       <c r="C4" s="174" t="n"/>
       <c r="D4" s="175" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E4" s="177" t="inlineStr">
         <is>
@@ -3881,9 +3881,7 @@
       </c>
       <c r="B6" s="160" t="n"/>
       <c r="C6" s="160" t="n"/>
-      <c r="D6" s="226" t="n">
-        <v>3</v>
-      </c>
+      <c r="D6" s="226" t="n"/>
       <c r="E6" s="219" t="n"/>
       <c r="F6" s="223" t="n"/>
       <c r="G6" s="227" t="inlineStr">
@@ -3894,9 +3892,7 @@
       <c r="H6" s="219" t="n"/>
       <c r="I6" s="219" t="n"/>
       <c r="J6" s="223" t="n"/>
-      <c r="K6" s="222" t="n">
-        <v>2</v>
-      </c>
+      <c r="K6" s="222" t="n"/>
       <c r="L6" s="219" t="n"/>
       <c r="M6" s="219" t="n"/>
       <c r="N6" s="219" t="n"/>
@@ -3909,9 +3905,7 @@
       </c>
       <c r="R6" s="160" t="n"/>
       <c r="S6" s="161" t="n"/>
-      <c r="T6" s="222" t="n">
-        <v>2</v>
-      </c>
+      <c r="T6" s="222" t="n"/>
       <c r="U6" s="219" t="n"/>
       <c r="V6" s="219" t="n"/>
       <c r="W6" s="219" t="n"/>
@@ -3984,7 +3978,7 @@
       <c r="C8" s="161" t="n"/>
       <c r="D8" s="209" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>Standard Rooms Only2</t>
         </is>
       </c>
       <c r="E8" s="210" t="n"/>
@@ -4119,14 +4113,9 @@
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="255" t="inlineStr">
         <is>
-          <t>"SIMULATEUR DE LEVAGE DE LA PAZ
-Entraîne les muscles extenseurs de manière sûre et efficace en position horizontale. Le coussin rond parfaitement formé et ajustable ainsi que le réglage individuel de la longueur des jambes créent une situation optimale pour l’entraînement.
-Hauteur: 1570 mm
-Largeur: 1200 mm
-Longueur: 1800 mm
-Poids total 290.00 kg
-Bloc de poids standard 60 kg
-Qty: 1 U"</t>
+          <t>"RACK POUR LES GRIFFE EXCLUSIVES RAUSCHENBACH
+Qty: 1 U
+"</t>
         </is>
       </c>
       <c r="B11" s="256" t="n"/>
@@ -4142,13 +4131,7 @@
       <c r="L11" s="98" t="n"/>
       <c r="M11" s="260" t="inlineStr">
         <is>
-          <t>"ТРЕНАЖЕР ДЛЯ ПОДЪЕМА ТАЗА
-Тренирует мышцы-разгибатели безопасно и эффективно в горизонтальном положении. Идеальная форма и регулируемая круглая подушка, а также индивидуальная регулировка длины ног создают оптимальную тренировочную ситуацию.
-Высота: 1570 мм
-Ширина: 1200 мм
-Длина: 1800 мм
-Общий вес 290,00 кг
-Стандартный вес блока 60 кг
+          <t>"СТОЙКА ДЛЯ ГРИФОВ ЭКСКЛЮЗИВНОЙ КОНСТРУКЦИИ RAUSCHENBACH
 Кол-во: 1 шт"</t>
         </is>
       </c>
@@ -4747,11 +4730,7 @@
       <c r="B29" s="160" t="n"/>
       <c r="C29" s="160" t="n"/>
       <c r="D29" s="217" t="n"/>
-      <c r="E29" s="242" t="inlineStr">
-        <is>
-          <t>Some Protocol</t>
-        </is>
-      </c>
+      <c r="E29" s="242" t="inlineStr"/>
       <c r="F29" s="219" t="n"/>
       <c r="G29" s="219" t="n"/>
       <c r="H29" s="219" t="n"/>
@@ -4830,11 +4809,7 @@
       <c r="B31" s="160" t="n"/>
       <c r="C31" s="160" t="n"/>
       <c r="D31" s="160" t="n"/>
-      <c r="E31" s="242" t="inlineStr">
-        <is>
-          <t>Good observation</t>
-        </is>
-      </c>
+      <c r="E31" s="242" t="inlineStr"/>
       <c r="F31" s="219" t="n"/>
       <c r="G31" s="219" t="n"/>
       <c r="H31" s="219" t="n"/>
@@ -5412,13 +5387,11 @@
       <c r="B45" s="297" t="n"/>
       <c r="C45" s="297" t="n"/>
       <c r="D45" s="298" t="n"/>
-      <c r="E45" s="163" t="n">
-        <v>2</v>
-      </c>
+      <c r="E45" s="163" t="n"/>
       <c r="F45" s="164" t="n"/>
       <c r="G45" s="165" t="n"/>
       <c r="H45" s="299" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="I45" s="298" t="n"/>
       <c r="J45" s="166" t="n"/>
@@ -5431,18 +5404,14 @@
       <c r="Q45" s="168" t="n"/>
       <c r="R45" s="167" t="inlineStr">
         <is>
-          <t>04003</t>
+          <t>70112</t>
         </is>
       </c>
       <c r="S45" s="301" t="n"/>
       <c r="T45" s="301" t="n"/>
       <c r="U45" s="301" t="n"/>
       <c r="V45" s="168" t="n"/>
-      <c r="W45" s="300" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
+      <c r="W45" s="300" t="inlineStr"/>
       <c r="X45" s="301" t="n"/>
       <c r="Y45" s="302" t="n"/>
       <c r="Z45" s="283" t="n"/>

</xml_diff>

<commit_message>
edit/detail/print templates are working
</commit_message>
<xml_diff>
--- a/media/excel_template/fp_temp.xlsx
+++ b/media/excel_template/fp_temp.xlsx
@@ -3231,12 +3231,12 @@
   </twoCellAnchor>
   <oneCellAnchor>
     <from>
-      <col>6</col>
+      <col>7</col>
       <colOff>304919</colOff>
       <row>22</row>
       <rowOff>90490</rowOff>
     </from>
-    <ext cx="2895600" cy="2333625"/>
+    <ext cx="2514600" cy="2333625"/>
     <pic>
       <nvPicPr>
         <cNvPr id="2" name="Image 2" descr="Picture"/>
@@ -3718,7 +3718,7 @@
       <c r="F2" s="196" t="n"/>
       <c r="G2" s="197" t="inlineStr">
         <is>
-          <t>RACK POUR LES GRIFFE EXCLUSIVES RAUSCHENBACH</t>
+          <t>MACHINE D'EXERCICE POUR L'ENTRAINEMENT DES MUSCLES DU MOLLET</t>
         </is>
       </c>
       <c r="H2" s="179" t="n"/>
@@ -3759,7 +3759,7 @@
       <c r="F3" s="199" t="n"/>
       <c r="G3" s="200" t="inlineStr">
         <is>
-          <t>СТОЙКА ДЛЯ ГРИФОВ ЭКСКЛЮЗИВНОЙ КОНСТРУКЦИИ RAUSCHENBACH</t>
+          <t>ТРЕНАЖЕР ДЛЯ ТРЕНИРОВКИ ИКРОНОЖНЫХ МЫШЦ</t>
         </is>
       </c>
       <c r="H3" s="201" t="n"/>
@@ -3806,7 +3806,7 @@
       <c r="B4" s="174" t="n"/>
       <c r="C4" s="174" t="n"/>
       <c r="D4" s="175" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E4" s="177" t="inlineStr">
         <is>
@@ -3881,7 +3881,9 @@
       </c>
       <c r="B6" s="160" t="n"/>
       <c r="C6" s="160" t="n"/>
-      <c r="D6" s="226" t="n"/>
+      <c r="D6" s="226" t="n">
+        <v>2</v>
+      </c>
       <c r="E6" s="219" t="n"/>
       <c r="F6" s="223" t="n"/>
       <c r="G6" s="227" t="inlineStr">
@@ -3892,7 +3894,9 @@
       <c r="H6" s="219" t="n"/>
       <c r="I6" s="219" t="n"/>
       <c r="J6" s="223" t="n"/>
-      <c r="K6" s="222" t="n"/>
+      <c r="K6" s="222" t="n">
+        <v>5</v>
+      </c>
       <c r="L6" s="219" t="n"/>
       <c r="M6" s="219" t="n"/>
       <c r="N6" s="219" t="n"/>
@@ -3905,7 +3909,9 @@
       </c>
       <c r="R6" s="160" t="n"/>
       <c r="S6" s="161" t="n"/>
-      <c r="T6" s="222" t="n"/>
+      <c r="T6" s="222" t="n">
+        <v>5</v>
+      </c>
       <c r="U6" s="219" t="n"/>
       <c r="V6" s="219" t="n"/>
       <c r="W6" s="219" t="n"/>
@@ -3976,11 +3982,7 @@
       </c>
       <c r="B8" s="160" t="n"/>
       <c r="C8" s="161" t="n"/>
-      <c r="D8" s="209" t="inlineStr">
-        <is>
-          <t>Standard Rooms Only2</t>
-        </is>
-      </c>
+      <c r="D8" s="209" t="n"/>
       <c r="E8" s="210" t="n"/>
       <c r="F8" s="210" t="n"/>
       <c r="G8" s="210" t="n"/>
@@ -4113,9 +4115,8 @@
     <row r="11" ht="12.75" customHeight="1">
       <c r="A11" s="255" t="inlineStr">
         <is>
-          <t>"RACK POUR LES GRIFFE EXCLUSIVES RAUSCHENBACH
-Qty: 1 U
-"</t>
+          <t>"MACHINE D'EXERCICE POUR L'ENTRAINEMENT DES MUSCLES DU MOLLET                                                                                                Entraîne efficacement et en toute sécurité les muscles du mollet. À cet égard, le coussin de siège de forme anatomique ainsi que le siège en luge réglable pour une adaptation de la longueur des jambes garantissent toujours une biomécanique optimale. Grâce à la position du siège, la colonne vertébrale est déchargée. Tout cela garantit un entraînement confortable et sûr. Ceci est confirmé et documenté par l'homologation de la machine en tant que ""produit médical"" conformément à MPG.                             
+Qté:1"</t>
         </is>
       </c>
       <c r="B11" s="256" t="n"/>
@@ -4131,8 +4132,10 @@
       <c r="L11" s="98" t="n"/>
       <c r="M11" s="260" t="inlineStr">
         <is>
-          <t>"СТОЙКА ДЛЯ ГРИФОВ ЭКСКЛЮЗИВНОЙ КОНСТРУКЦИИ RAUSCHENBACH
-Кол-во: 1 шт"</t>
+          <t>"ТРЕНАЖЕР ДЛЯ ТРЕНИРОВКИ ИКРОНОЖНЫХ МЫШЦ
+Эффективно и безопасно тренирует икроножные мышцы. В этом отношении подушка сиденья анатомической формы и регулируемое сиденье салазок для адаптации длины ноги всегда гарантируют оптимальную биомеханику. Из-за положения сиденья позвоночник разгружен. Все это гарантирует комфортную и безопасную тренировку. Это подтверждается и документируется утверждением машины как «медицинского продукта» согласно MPG.
+Кол-во: 1 шт             
+"</t>
         </is>
       </c>
       <c r="N11" s="256" t="n"/>
@@ -4730,7 +4733,7 @@
       <c r="B29" s="160" t="n"/>
       <c r="C29" s="160" t="n"/>
       <c r="D29" s="217" t="n"/>
-      <c r="E29" s="242" t="inlineStr"/>
+      <c r="E29" s="242" t="n"/>
       <c r="F29" s="219" t="n"/>
       <c r="G29" s="219" t="n"/>
       <c r="H29" s="219" t="n"/>
@@ -4809,7 +4812,7 @@
       <c r="B31" s="160" t="n"/>
       <c r="C31" s="160" t="n"/>
       <c r="D31" s="160" t="n"/>
-      <c r="E31" s="242" t="inlineStr"/>
+      <c r="E31" s="242" t="n"/>
       <c r="F31" s="219" t="n"/>
       <c r="G31" s="219" t="n"/>
       <c r="H31" s="219" t="n"/>
@@ -5387,14 +5390,18 @@
       <c r="B45" s="297" t="n"/>
       <c r="C45" s="297" t="n"/>
       <c r="D45" s="298" t="n"/>
-      <c r="E45" s="163" t="n"/>
+      <c r="E45" s="163" t="n">
+        <v>2</v>
+      </c>
       <c r="F45" s="164" t="n"/>
       <c r="G45" s="165" t="n"/>
       <c r="H45" s="299" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="I45" s="298" t="n"/>
-      <c r="J45" s="166" t="n"/>
+      <c r="J45" s="166" t="n">
+        <v>1</v>
+      </c>
       <c r="K45" s="164" t="n"/>
       <c r="L45" s="164" t="n"/>
       <c r="M45" s="165" t="n"/>
@@ -5404,14 +5411,18 @@
       <c r="Q45" s="168" t="n"/>
       <c r="R45" s="167" t="inlineStr">
         <is>
-          <t>70112</t>
+          <t>03002</t>
         </is>
       </c>
       <c r="S45" s="301" t="n"/>
       <c r="T45" s="301" t="n"/>
       <c r="U45" s="301" t="n"/>
       <c r="V45" s="168" t="n"/>
-      <c r="W45" s="300" t="inlineStr"/>
+      <c r="W45" s="300" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
       <c r="X45" s="301" t="n"/>
       <c r="Y45" s="302" t="n"/>
       <c r="Z45" s="283" t="n"/>

</xml_diff>